<commit_message>
USBR aggregated data update.
</commit_message>
<xml_diff>
--- a/USBR/Colorado River Basin Natural Flow and Salt Data/Summary Sheet/AggregatedAmounts/RawInputData/byState/USBR_Tri.xlsx
+++ b/USBR/Colorado River Basin Natural Flow and Salt Data/Summary Sheet/AggregatedAmounts/RawInputData/byState/USBR_Tri.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="44">
   <si>
     <t>OBJECTID</t>
   </si>
@@ -91,13 +91,19 @@
     <t>2017-04-17</t>
   </si>
   <si>
-    <t>UT,WY</t>
-  </si>
-  <si>
-    <t>AZ,CO,NM,UT</t>
-  </si>
-  <si>
-    <t>CO,UT</t>
+    <t>CO</t>
+  </si>
+  <si>
+    <t>AZ</t>
+  </si>
+  <si>
+    <t>WY</t>
+  </si>
+  <si>
+    <t>UT</t>
+  </si>
+  <si>
+    <t>NM</t>
   </si>
   <si>
     <t>1404010703</t>
@@ -585,13 +591,13 @@
         <v>25</v>
       </c>
       <c r="L2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="M2" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="N2" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="P2">
         <v>2.29424818947</v>
@@ -600,7 +606,7 @@
         <v>0.09004617916</v>
       </c>
       <c r="R2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:18">
@@ -626,7 +632,7 @@
         <v>26</v>
       </c>
       <c r="M3" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="P3">
         <v>18.3651101103</v>
@@ -635,7 +641,7 @@
         <v>6.52057597573</v>
       </c>
       <c r="R3" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:18">
@@ -658,10 +664,10 @@
         <v>25480.46</v>
       </c>
       <c r="K4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="M4" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="P4">
         <v>13.2952780833</v>
@@ -670,7 +676,7 @@
         <v>2.67164602838</v>
       </c>
       <c r="R4" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:18">
@@ -696,16 +702,16 @@
         <v>840.3200000000001</v>
       </c>
       <c r="K5" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="L5" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="M5" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="N5" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="P5">
         <v>2.29424818947</v>
@@ -714,7 +720,7 @@
         <v>0.09004617916</v>
       </c>
       <c r="R5" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:18">
@@ -740,16 +746,16 @@
         <v>840.3200000000001</v>
       </c>
       <c r="K6" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="L6" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="M6" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="N6" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="P6">
         <v>2.29424818947</v>
@@ -758,7 +764,7 @@
         <v>0.09004617916</v>
       </c>
       <c r="R6" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
     </row>
     <row r="7" spans="1:18">
@@ -781,10 +787,10 @@
         <v>25480.46</v>
       </c>
       <c r="K7" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="M7" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="P7">
         <v>13.2952780833</v>
@@ -793,7 +799,7 @@
         <v>2.67164602838</v>
       </c>
       <c r="R7" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:18">
@@ -816,10 +822,10 @@
         <v>64569.32</v>
       </c>
       <c r="K8" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="M8" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="P8">
         <v>18.3651101103</v>
@@ -828,7 +834,7 @@
         <v>6.52057597573</v>
       </c>
       <c r="R8" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
     </row>
     <row r="9" spans="1:18">
@@ -851,10 +857,10 @@
         <v>64569.32</v>
       </c>
       <c r="K9" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="M9" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="P9">
         <v>18.3651101103</v>
@@ -863,7 +869,7 @@
         <v>6.52057597573</v>
       </c>
       <c r="R9" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="10" spans="1:18">
@@ -886,10 +892,10 @@
         <v>64569.32</v>
       </c>
       <c r="K10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="M10" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="P10">
         <v>18.3651101103</v>
@@ -898,7 +904,7 @@
         <v>6.52057597573</v>
       </c>
       <c r="R10" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>